<commit_message>
Rhythm Machine Main Board PSoC 5LP Prototyping Kit Pin Assign ピンアサインを変更
</commit_message>
<xml_diff>
--- a/Master_PSoC5LP_Test/PSoC/Rhythm Machine Main Board PSoC 5LP Prototyping Kit Pin Assign.xlsx
+++ b/Master_PSoC5LP_Test/PSoC/Rhythm Machine Main Board PSoC 5LP Prototyping Kit Pin Assign.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t xml:space="preserve">Rhythm Machine Main Board </t>
     <phoneticPr fontId="2"/>
@@ -154,12 +154,6 @@
   </si>
   <si>
     <t>Pin_SW2_in</t>
-  </si>
-  <si>
-    <t>Pin_SW3_in</t>
-  </si>
-  <si>
-    <t>Pin_SW4_in</t>
   </si>
   <si>
     <t>Pin_RE1_in[0]</t>
@@ -370,23 +364,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -685,7 +679,7 @@
   <dimension ref="B2:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -721,27 +715,27 @@
       <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13" t="s">
+      <c r="D6" s="18"/>
+      <c r="E6" s="12" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13" t="s">
+      <c r="I6" s="18"/>
+      <c r="J6" s="12" t="s">
         <v>27</v>
       </c>
       <c r="L6" s="1"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="13"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="12"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7">
@@ -774,7 +768,7 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>34</v>
       </c>
       <c r="G8">
@@ -785,8 +779,8 @@
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="3"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
       <c r="O8" s="11"/>
     </row>
     <row r="9" spans="2:15">
@@ -811,8 +805,8 @@
       <c r="I9">
         <v>7</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>9</v>
+      <c r="J9" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="O9" s="11"/>
     </row>
@@ -826,9 +820,7 @@
       <c r="D10">
         <v>2</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="E10" s="11"/>
       <c r="G10">
         <v>49</v>
       </c>
@@ -838,8 +830,8 @@
       <c r="I10">
         <v>6</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>10</v>
+      <c r="J10" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="O10" s="11"/>
     </row>
@@ -853,9 +845,7 @@
       <c r="D11">
         <v>3</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="E11" s="11"/>
       <c r="G11">
         <v>48</v>
       </c>
@@ -966,14 +956,14 @@
       <c r="B16">
         <v>10</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="15">
         <v>0</v>
       </c>
-      <c r="E16" s="18" t="s">
-        <v>38</v>
+      <c r="E16" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="G16">
         <v>43</v>
@@ -992,14 +982,14 @@
       <c r="B17">
         <v>11</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="15">
         <v>1</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G17">
         <v>42</v>
@@ -1019,14 +1009,14 @@
       <c r="B18">
         <v>12</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="15">
         <v>2</v>
       </c>
-      <c r="E18" s="18" t="s">
-        <v>40</v>
+      <c r="E18" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="G18">
         <v>41</v>
@@ -1046,14 +1036,14 @@
       <c r="B19">
         <v>13</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="15">
         <v>3</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G19">
         <v>40</v>
@@ -1073,14 +1063,14 @@
       <c r="B20">
         <v>14</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="15">
         <v>4</v>
       </c>
-      <c r="E20" s="18" t="s">
-        <v>42</v>
+      <c r="E20" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="G20">
         <v>39</v>
@@ -1100,14 +1090,14 @@
       <c r="B21">
         <v>15</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="15">
         <v>5</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G21">
         <v>38</v>
@@ -1127,10 +1117,10 @@
       <c r="B22">
         <v>16</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="15">
         <v>0</v>
       </c>
       <c r="E22" s="11"/>
@@ -1143,8 +1133,8 @@
       <c r="I22">
         <v>5</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>17</v>
+      <c r="J22" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="O22" s="11"/>
     </row>
@@ -1152,10 +1142,10 @@
       <c r="B23">
         <v>17</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="15">
         <v>1</v>
       </c>
       <c r="E23" s="11"/>
@@ -1177,10 +1167,10 @@
       <c r="B24">
         <v>18</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="15">
         <v>2</v>
       </c>
       <c r="E24" s="11"/>
@@ -1193,8 +1183,8 @@
       <c r="I24">
         <v>7</v>
       </c>
-      <c r="J24" s="8" t="s">
-        <v>19</v>
+      <c r="J24" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="O24" s="11"/>
     </row>
@@ -1202,10 +1192,10 @@
       <c r="B25">
         <v>19</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="15">
         <v>3</v>
       </c>
       <c r="E25" s="11"/>
@@ -1224,10 +1214,10 @@
       <c r="B26">
         <v>20</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="15">
         <v>4</v>
       </c>
       <c r="E26" s="11"/>
@@ -1249,10 +1239,10 @@
       <c r="B27">
         <v>21</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="15">
         <v>5</v>
       </c>
       <c r="E27" s="11"/>
@@ -1274,14 +1264,14 @@
       <c r="B28">
         <v>22</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="15">
         <v>6</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G28">
         <v>31</v>
@@ -1301,14 +1291,14 @@
       <c r="B29">
         <v>23</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="15">
         <v>7</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G29">
         <v>30</v>
@@ -1365,7 +1355,7 @@
       <c r="I31">
         <v>1</v>
       </c>
-      <c r="J31" s="17" t="s">
+      <c r="J31" s="16" t="s">
         <v>25</v>
       </c>
       <c r="O31" s="11"/>
@@ -1378,7 +1368,7 @@
         <v>30</v>
       </c>
       <c r="D32" s="2"/>
-      <c r="E32" s="15"/>
+      <c r="E32" s="14"/>
       <c r="G32">
         <v>27</v>
       </c>
@@ -1391,7 +1381,7 @@
       <c r="J32" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="O32" s="14"/>
+      <c r="O32" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Rhythm Machine Main Board PSoC 5LP Prototyping Kit Pin Assign.xlsxを更新
</commit_message>
<xml_diff>
--- a/Master_PSoC5LP_Test/PSoC/Rhythm Machine Main Board PSoC 5LP Prototyping Kit Pin Assign.xlsx
+++ b/Master_PSoC5LP_Test/PSoC/Rhythm Machine Main Board PSoC 5LP Prototyping Kit Pin Assign.xlsx
@@ -62,26 +62,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Pin_SCK</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Pin_MISO</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Pin_MOSI</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Pin_SS1</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Pin_SS2</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>LED_RED</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -194,7 +174,27 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>2015.11.20</t>
+    <t>2015.11.24</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Pin_SPI_SCK</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Pin_SPI_MISO</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Pin_SPI_MOSI</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Pin_SPI_Ex1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Pin_SPI Ex2</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -720,29 +720,29 @@
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:15">
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>2</v>
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="18"/>
@@ -775,13 +775,13 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G8">
         <v>51</v>
@@ -800,13 +800,13 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G9">
         <v>50</v>
@@ -827,7 +827,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -852,13 +852,13 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>43</v>
+      <c r="E11" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="G11">
         <v>48</v>
@@ -879,13 +879,13 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>44</v>
+      <c r="E12" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="G12">
         <v>47</v>
@@ -903,13 +903,13 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D13">
         <v>5</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>45</v>
+      <c r="E13" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="G13">
         <v>46</v>
@@ -929,7 +929,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -951,7 +951,7 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D15">
         <v>7</v>
@@ -975,13 +975,13 @@
         <v>10</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D16" s="15">
         <v>0</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G16">
         <v>43</v>
@@ -1001,13 +1001,13 @@
         <v>11</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D17" s="15">
         <v>1</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G17">
         <v>42</v>
@@ -1019,7 +1019,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="O17" s="11"/>
     </row>
@@ -1028,13 +1028,13 @@
         <v>12</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D18" s="15">
         <v>2</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G18">
         <v>41</v>
@@ -1046,7 +1046,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="O18" s="11"/>
     </row>
@@ -1055,13 +1055,13 @@
         <v>13</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D19" s="15">
         <v>3</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G19">
         <v>40</v>
@@ -1073,7 +1073,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="O19" s="11"/>
     </row>
@@ -1082,13 +1082,13 @@
         <v>14</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D20" s="15">
         <v>4</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G20">
         <v>39</v>
@@ -1100,7 +1100,7 @@
         <v>3</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="O20" s="11"/>
     </row>
@@ -1109,13 +1109,13 @@
         <v>15</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D21" s="15">
         <v>5</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G21">
         <v>38</v>
@@ -1127,7 +1127,7 @@
         <v>4</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="O21" s="11"/>
     </row>
@@ -1136,7 +1136,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D22" s="15">
         <v>0</v>
@@ -1152,7 +1152,7 @@
         <v>5</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="O22" s="11"/>
     </row>
@@ -1161,7 +1161,7 @@
         <v>17</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D23" s="15">
         <v>1</v>
@@ -1177,7 +1177,7 @@
         <v>6</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="O23" s="11"/>
     </row>
@@ -1186,7 +1186,7 @@
         <v>18</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D24" s="15">
         <v>2</v>
@@ -1202,7 +1202,7 @@
         <v>7</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="O24" s="11"/>
     </row>
@@ -1211,7 +1211,7 @@
         <v>19</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D25" s="15">
         <v>3</v>
@@ -1233,7 +1233,7 @@
         <v>20</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D26" s="15">
         <v>4</v>
@@ -1249,7 +1249,7 @@
         <v>6</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="O26" s="11"/>
     </row>
@@ -1258,7 +1258,7 @@
         <v>21</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D27" s="15">
         <v>5</v>
@@ -1274,7 +1274,7 @@
         <v>5</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="O27" s="11"/>
     </row>
@@ -1283,13 +1283,13 @@
         <v>22</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D28" s="15">
         <v>6</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G28">
         <v>31</v>
@@ -1301,7 +1301,7 @@
         <v>4</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="O28" s="11"/>
     </row>
@@ -1310,13 +1310,13 @@
         <v>23</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D29" s="15">
         <v>7</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G29">
         <v>30</v>
@@ -1328,7 +1328,7 @@
         <v>3</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="O29" s="11"/>
     </row>
@@ -1337,7 +1337,7 @@
         <v>24</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -1351,7 +1351,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="O30" s="11"/>
     </row>
@@ -1374,7 +1374,7 @@
         <v>1</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="O31" s="11"/>
     </row>
@@ -1383,7 +1383,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="14"/>
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="O32" s="13"/>
     </row>

</xml_diff>